<commit_message>
- added SOTA approach and updated results and figures
</commit_message>
<xml_diff>
--- a/TestResultsEEG.xlsx
+++ b/TestResultsEEG.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana Leal\Documents\GitHub\SeizurePrediction\Results\figures_paper_threshold_redundance90_th_0.7_gm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adriana Leal\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2447929F-1750-4DC1-ABAF-A6D70A441E39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{863C13AF-5CFC-4E09-A44E-4242FF1CF6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1920" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hybrid" sheetId="1" r:id="rId1"/>
-    <sheet name="Control" sheetId="2" r:id="rId2"/>
+    <sheet name="Control" sheetId="3" r:id="rId2"/>
+    <sheet name="SOTA" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="197">
   <si>
     <t>Patient</t>
   </si>
@@ -77,7 +78,7 @@
     <t>AUC</t>
   </si>
   <si>
-    <t>0.67±0.47</t>
+    <t>0.71±0.46</t>
   </si>
   <si>
     <t>16202</t>
@@ -122,415 +123,466 @@
     <t>32.66</t>
   </si>
   <si>
+    <t>0.11±0.31</t>
+  </si>
+  <si>
+    <t>30802</t>
+  </si>
+  <si>
+    <t>61.19</t>
+  </si>
+  <si>
+    <t>16.42</t>
+  </si>
+  <si>
+    <t>0.41±0.49</t>
+  </si>
+  <si>
+    <t>32702</t>
+  </si>
+  <si>
+    <t>34.73</t>
+  </si>
+  <si>
+    <t>7.45</t>
+  </si>
+  <si>
+    <t>45402</t>
+  </si>
+  <si>
+    <t>24.94</t>
+  </si>
+  <si>
+    <t>0.06±0.23</t>
+  </si>
+  <si>
+    <t>46702</t>
+  </si>
+  <si>
+    <t>0.08±0.27</t>
+  </si>
+  <si>
+    <t>50802</t>
+  </si>
+  <si>
+    <t>40.0</t>
+  </si>
+  <si>
+    <t>0.0</t>
+  </si>
+  <si>
+    <t>0.07±0.25</t>
+  </si>
+  <si>
+    <t>52302</t>
+  </si>
+  <si>
+    <t>53402</t>
+  </si>
+  <si>
+    <t>37.53</t>
+  </si>
+  <si>
+    <t>10.25</t>
+  </si>
+  <si>
+    <t>0.21±0.41</t>
+  </si>
+  <si>
+    <t>55202</t>
+  </si>
+  <si>
+    <t>57.48</t>
+  </si>
+  <si>
+    <t>16.72</t>
+  </si>
+  <si>
+    <t>0.12±0.33</t>
+  </si>
+  <si>
+    <t>56402</t>
+  </si>
+  <si>
+    <t>72.08</t>
+  </si>
+  <si>
+    <t>5.83</t>
+  </si>
+  <si>
+    <t>0.16±0.37</t>
+  </si>
+  <si>
+    <t>58602</t>
+  </si>
+  <si>
+    <t>58.86</t>
+  </si>
+  <si>
+    <t>18.3</t>
+  </si>
+  <si>
+    <t>0.44±0.5</t>
+  </si>
+  <si>
+    <t>59102</t>
+  </si>
+  <si>
+    <t>93.56</t>
+  </si>
+  <si>
+    <t>0.72±0.45</t>
+  </si>
+  <si>
+    <t>60002</t>
+  </si>
+  <si>
+    <t>39.95</t>
+  </si>
+  <si>
+    <t>7.35</t>
+  </si>
+  <si>
+    <t>64702</t>
+  </si>
+  <si>
+    <t>57.91</t>
+  </si>
+  <si>
+    <t>29.99</t>
+  </si>
+  <si>
+    <t>0.15±0.36</t>
+  </si>
+  <si>
+    <t>75202</t>
+  </si>
+  <si>
+    <t>54.97</t>
+  </si>
+  <si>
+    <t>27.45</t>
+  </si>
+  <si>
+    <t>0.06±0.24</t>
+  </si>
+  <si>
+    <t>80702</t>
+  </si>
+  <si>
+    <t>56.46</t>
+  </si>
+  <si>
+    <t>20.82</t>
+  </si>
+  <si>
+    <t>85202</t>
+  </si>
+  <si>
+    <t>77.87</t>
+  </si>
+  <si>
+    <t>31.5</t>
+  </si>
+  <si>
+    <t>0.09±0.28</t>
+  </si>
+  <si>
+    <t>93402</t>
+  </si>
+  <si>
+    <t>0.6±0.49</t>
+  </si>
+  <si>
+    <t>93902</t>
+  </si>
+  <si>
+    <t>44.33</t>
+  </si>
+  <si>
+    <t>11.44</t>
+  </si>
+  <si>
+    <t>0.05±0.21</t>
+  </si>
+  <si>
+    <t>94402</t>
+  </si>
+  <si>
+    <t>54.11</t>
+  </si>
+  <si>
+    <t>26.04</t>
+  </si>
+  <si>
+    <t>95202</t>
+  </si>
+  <si>
+    <t>36.56</t>
+  </si>
+  <si>
+    <t>4.86</t>
+  </si>
+  <si>
+    <t>0.27±0.44</t>
+  </si>
+  <si>
+    <t>96002</t>
+  </si>
+  <si>
+    <t>73.22</t>
+  </si>
+  <si>
+    <t>40.86</t>
+  </si>
+  <si>
+    <t>0.32±0.47</t>
+  </si>
+  <si>
+    <t>98102</t>
+  </si>
+  <si>
+    <t>104.29</t>
+  </si>
+  <si>
+    <t>11.48</t>
+  </si>
+  <si>
+    <t>0.06±0.25</t>
+  </si>
+  <si>
+    <t>98202</t>
+  </si>
+  <si>
+    <t>68.5</t>
+  </si>
+  <si>
+    <t>36.49</t>
+  </si>
+  <si>
+    <t>0.71±0.45</t>
+  </si>
+  <si>
+    <t>101702</t>
+  </si>
+  <si>
+    <t>96.82</t>
+  </si>
+  <si>
+    <t>32.78</t>
+  </si>
+  <si>
+    <t>0.07±0.26</t>
+  </si>
+  <si>
+    <t>102202</t>
+  </si>
+  <si>
+    <t>85.92</t>
+  </si>
+  <si>
+    <t>33.72</t>
+  </si>
+  <si>
+    <t>0.02±0.14</t>
+  </si>
+  <si>
+    <t>104602</t>
+  </si>
+  <si>
+    <t>66.67</t>
+  </si>
+  <si>
+    <t>37.71</t>
+  </si>
+  <si>
+    <t>0.39±0.49</t>
+  </si>
+  <si>
+    <t>109502</t>
+  </si>
+  <si>
+    <t>38.24</t>
+  </si>
+  <si>
+    <t>15.75</t>
+  </si>
+  <si>
+    <t>0.64±0.48</t>
+  </si>
+  <si>
+    <t>110602</t>
+  </si>
+  <si>
+    <t>0.25±0.44</t>
+  </si>
+  <si>
+    <t>112802</t>
+  </si>
+  <si>
+    <t>38.73</t>
+  </si>
+  <si>
+    <t>1.8</t>
+  </si>
+  <si>
+    <t>0.49±0.5</t>
+  </si>
+  <si>
+    <t>113902</t>
+  </si>
+  <si>
+    <t>46.89</t>
+  </si>
+  <si>
+    <t>24.07</t>
+  </si>
+  <si>
+    <t>114702</t>
+  </si>
+  <si>
+    <t>63.32</t>
+  </si>
+  <si>
+    <t>28.69</t>
+  </si>
+  <si>
+    <t>0.09±0.29</t>
+  </si>
+  <si>
+    <t>114902</t>
+  </si>
+  <si>
+    <t>123902</t>
+  </si>
+  <si>
+    <t>41.77</t>
+  </si>
+  <si>
+    <t>2.51</t>
+  </si>
+  <si>
+    <t>93.33</t>
+  </si>
+  <si>
+    <t>120.0</t>
+  </si>
+  <si>
+    <t>0.11±0.32</t>
+  </si>
+  <si>
+    <t>60.0</t>
+  </si>
+  <si>
+    <t>16.33</t>
+  </si>
+  <si>
     <t>0.1±0.3</t>
   </si>
   <si>
-    <t>30802</t>
-  </si>
-  <si>
-    <t>61.19</t>
-  </si>
-  <si>
-    <t>16.42</t>
-  </si>
-  <si>
-    <t>0.41±0.49</t>
-  </si>
-  <si>
-    <t>32702</t>
-  </si>
-  <si>
-    <t>34.73</t>
-  </si>
-  <si>
-    <t>7.45</t>
-  </si>
-  <si>
-    <t>45402</t>
-  </si>
-  <si>
-    <t>24.94</t>
-  </si>
-  <si>
-    <t>0.06±0.23</t>
-  </si>
-  <si>
-    <t>46702</t>
-  </si>
-  <si>
-    <t>0.09±0.28</t>
-  </si>
-  <si>
-    <t>50802</t>
-  </si>
-  <si>
-    <t>40.0</t>
-  </si>
-  <si>
-    <t>0.0</t>
-  </si>
-  <si>
-    <t>0.07±0.26</t>
-  </si>
-  <si>
-    <t>52302</t>
-  </si>
-  <si>
-    <t>0.38±0.49</t>
-  </si>
-  <si>
-    <t>53402</t>
-  </si>
-  <si>
-    <t>37.53</t>
-  </si>
-  <si>
-    <t>10.25</t>
-  </si>
-  <si>
-    <t>55202</t>
-  </si>
-  <si>
-    <t>57.48</t>
-  </si>
-  <si>
-    <t>16.72</t>
-  </si>
-  <si>
-    <t>0.12±0.33</t>
-  </si>
-  <si>
-    <t>56402</t>
-  </si>
-  <si>
-    <t>72.08</t>
-  </si>
-  <si>
-    <t>5.83</t>
-  </si>
-  <si>
-    <t>0.16±0.37</t>
-  </si>
-  <si>
-    <t>58602</t>
-  </si>
-  <si>
-    <t>58.86</t>
-  </si>
-  <si>
-    <t>18.3</t>
-  </si>
-  <si>
-    <t>0.44±0.5</t>
-  </si>
-  <si>
-    <t>59102</t>
-  </si>
-  <si>
-    <t>93.56</t>
-  </si>
-  <si>
-    <t>0.73±0.44</t>
-  </si>
-  <si>
-    <t>60002</t>
-  </si>
-  <si>
-    <t>39.95</t>
-  </si>
-  <si>
-    <t>7.35</t>
-  </si>
-  <si>
-    <t>64702</t>
-  </si>
-  <si>
-    <t>57.91</t>
-  </si>
-  <si>
-    <t>29.99</t>
+    <t>53.33</t>
+  </si>
+  <si>
+    <t>9.43</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>0.4±0.49</t>
+  </si>
+  <si>
+    <t>0.74±0.44</t>
+  </si>
+  <si>
+    <t>46.67</t>
+  </si>
+  <si>
+    <t>0.51±0.5</t>
+  </si>
+  <si>
+    <t>0.03±0.16</t>
+  </si>
+  <si>
+    <t>0.84±0.37</t>
+  </si>
+  <si>
+    <t>0.24±0.43</t>
+  </si>
+  <si>
+    <t>0.08±0.26</t>
+  </si>
+  <si>
+    <t>Frel</t>
+  </si>
+  <si>
+    <t>Fred</t>
+  </si>
+  <si>
+    <t>0.69±0.46</t>
+  </si>
+  <si>
+    <t>0.1±0.29</t>
+  </si>
+  <si>
+    <t>0.35±0.48</t>
   </si>
   <si>
     <t>0.17±0.37</t>
   </si>
   <si>
-    <t>75202</t>
-  </si>
-  <si>
-    <t>54.97</t>
-  </si>
-  <si>
-    <t>27.45</t>
-  </si>
-  <si>
-    <t>0.07±0.25</t>
-  </si>
-  <si>
-    <t>80702</t>
-  </si>
-  <si>
-    <t>56.46</t>
-  </si>
-  <si>
-    <t>20.82</t>
-  </si>
-  <si>
-    <t>0.43±0.49</t>
-  </si>
-  <si>
-    <t>85202</t>
-  </si>
-  <si>
-    <t>77.87</t>
-  </si>
-  <si>
-    <t>31.5</t>
-  </si>
-  <si>
-    <t>0.09±0.29</t>
-  </si>
-  <si>
-    <t>93402</t>
-  </si>
-  <si>
-    <t>0.61±0.49</t>
-  </si>
-  <si>
-    <t>93902</t>
-  </si>
-  <si>
-    <t>44.33</t>
-  </si>
-  <si>
-    <t>11.44</t>
-  </si>
-  <si>
-    <t>0.05±0.22</t>
-  </si>
-  <si>
-    <t>94402</t>
-  </si>
-  <si>
-    <t>54.11</t>
-  </si>
-  <si>
-    <t>26.04</t>
-  </si>
-  <si>
-    <t>95202</t>
-  </si>
-  <si>
-    <t>36.56</t>
-  </si>
-  <si>
-    <t>4.86</t>
-  </si>
-  <si>
-    <t>0.24±0.43</t>
-  </si>
-  <si>
-    <t>96002</t>
-  </si>
-  <si>
-    <t>73.22</t>
-  </si>
-  <si>
-    <t>40.86</t>
-  </si>
-  <si>
-    <t>0.31±0.46</t>
-  </si>
-  <si>
-    <t>98102</t>
-  </si>
-  <si>
-    <t>104.29</t>
-  </si>
-  <si>
-    <t>11.48</t>
-  </si>
-  <si>
-    <t>98202</t>
-  </si>
-  <si>
-    <t>68.5</t>
-  </si>
-  <si>
-    <t>36.49</t>
-  </si>
-  <si>
-    <t>0.72±0.45</t>
-  </si>
-  <si>
-    <t>101702</t>
-  </si>
-  <si>
-    <t>96.82</t>
-  </si>
-  <si>
-    <t>32.78</t>
-  </si>
-  <si>
-    <t>102202</t>
-  </si>
-  <si>
-    <t>85.92</t>
-  </si>
-  <si>
-    <t>33.72</t>
+    <t>0.02±0.15</t>
+  </si>
+  <si>
+    <t>0.04±0.2</t>
+  </si>
+  <si>
+    <t>0.54±0.5</t>
+  </si>
+  <si>
+    <t>0.34±0.48</t>
+  </si>
+  <si>
+    <t>0.08±0.28</t>
+  </si>
+  <si>
+    <t>0.76±0.43</t>
+  </si>
+  <si>
+    <t>0.03±0.18</t>
+  </si>
+  <si>
+    <t>0.5±0.5</t>
   </si>
   <si>
     <t>0.02±0.12</t>
   </si>
   <si>
-    <t>104602</t>
-  </si>
-  <si>
-    <t>66.67</t>
-  </si>
-  <si>
-    <t>37.71</t>
-  </si>
-  <si>
-    <t>0.39±0.49</t>
-  </si>
-  <si>
-    <t>109502</t>
-  </si>
-  <si>
-    <t>38.24</t>
-  </si>
-  <si>
-    <t>15.75</t>
+    <t>0.52±0.5</t>
+  </si>
+  <si>
+    <t>0.33±0.47</t>
+  </si>
+  <si>
+    <t>0.14±0.34</t>
   </si>
   <si>
     <t>0.62±0.49</t>
   </si>
   <si>
-    <t>110602</t>
-  </si>
-  <si>
-    <t>112802</t>
-  </si>
-  <si>
-    <t>38.73</t>
-  </si>
-  <si>
-    <t>1.8</t>
-  </si>
-  <si>
-    <t>0.47±0.5</t>
-  </si>
-  <si>
-    <t>113902</t>
-  </si>
-  <si>
-    <t>46.89</t>
-  </si>
-  <si>
-    <t>24.07</t>
-  </si>
-  <si>
-    <t>114702</t>
-  </si>
-  <si>
-    <t>63.32</t>
-  </si>
-  <si>
-    <t>28.69</t>
-  </si>
-  <si>
-    <t>114902</t>
-  </si>
-  <si>
-    <t>0.08±0.27</t>
-  </si>
-  <si>
-    <t>123902</t>
-  </si>
-  <si>
-    <t>41.77</t>
-  </si>
-  <si>
-    <t>2.51</t>
-  </si>
-  <si>
-    <t>93.33</t>
-  </si>
-  <si>
-    <t>0.66±0.47</t>
-  </si>
-  <si>
-    <t>120.0</t>
-  </si>
-  <si>
-    <t>0.11±0.32</t>
-  </si>
-  <si>
-    <t>0.12±0.32</t>
-  </si>
-  <si>
-    <t>60.0</t>
-  </si>
-  <si>
-    <t>16.33</t>
-  </si>
-  <si>
-    <t>0.06±0.24</t>
-  </si>
-  <si>
-    <t>53.33</t>
-  </si>
-  <si>
-    <t>9.43</t>
-  </si>
-  <si>
-    <t>100.0</t>
-  </si>
-  <si>
-    <t>0.4±0.49</t>
-  </si>
-  <si>
-    <t>0.74±0.44</t>
-  </si>
-  <si>
-    <t>0.02±0.13</t>
-  </si>
-  <si>
-    <t>0.03±0.17</t>
-  </si>
-  <si>
-    <t>46.67</t>
-  </si>
-  <si>
-    <t>0.51±0.5</t>
-  </si>
-  <si>
-    <t>0.21±0.41</t>
-  </si>
-  <si>
-    <t>0.34±0.47</t>
-  </si>
-  <si>
-    <t>0.75±0.43</t>
-  </si>
-  <si>
-    <t>0.03±0.16</t>
-  </si>
-  <si>
-    <t>0.84±0.37</t>
-  </si>
-  <si>
-    <t>0.49±0.5</t>
-  </si>
-  <si>
-    <t>0.25±0.44</t>
-  </si>
-  <si>
-    <t>0.02±0.14</t>
-  </si>
-  <si>
-    <t>0.08±0.26</t>
+    <t>0.3±0.46</t>
+  </si>
+  <si>
+    <t>0.45±0.5</t>
+  </si>
+  <si>
+    <t>0.26±0.44</t>
+  </si>
+  <si>
+    <t>0.48±0.5</t>
+  </si>
+  <si>
+    <t>0.63±0.48</t>
   </si>
   <si>
     <t># training seizures with unsupervised preictal</t>
@@ -552,12 +604,6 @@
   </si>
   <si>
     <t>FR method</t>
-  </si>
-  <si>
-    <t>Frel</t>
-  </si>
-  <si>
-    <t>Fred</t>
   </si>
   <si>
     <t>SS</t>
@@ -925,8 +971,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="N41" sqref="N41"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,49 +999,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -1092,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="O3" s="2">
-        <v>2.7699446392551569E-14</v>
+        <v>4.2271256758162232E-13</v>
       </c>
       <c r="P3" s="2">
         <v>1</v>
@@ -1142,7 +1188,7 @@
         <v>18</v>
       </c>
       <c r="O4" s="2">
-        <v>6.5376849652931543E-90</v>
+        <v>1.417559670517349E-77</v>
       </c>
       <c r="P4" s="2">
         <v>1</v>
@@ -1386,7 +1432,7 @@
         <v>37</v>
       </c>
       <c r="O9" s="2">
-        <v>5.8411682631609862E-160</v>
+        <v>2.9634362838058871E-152</v>
       </c>
       <c r="P9" s="2">
         <v>1</v>
@@ -1627,7 +1673,7 @@
         <v>1.7559255820265991</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2">
@@ -1636,7 +1682,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -1651,10 +1697,10 @@
         <v>0.09</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>7</v>
@@ -1675,7 +1721,7 @@
         <v>0.61062445471442905</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>8</v>
+        <v>54</v>
       </c>
       <c r="O15" s="2"/>
       <c r="P15" s="2">
@@ -1726,7 +1772,7 @@
         <v>58</v>
       </c>
       <c r="O16" s="2">
-        <v>4.9330861438619804E-65</v>
+        <v>1.981116115609267E-65</v>
       </c>
       <c r="P16" s="2">
         <v>1</v>
@@ -1872,7 +1918,7 @@
         <v>69</v>
       </c>
       <c r="O19" s="2">
-        <v>3.2931476549417578E-138</v>
+        <v>2.6372783132809261E-146</v>
       </c>
       <c r="P19" s="2">
         <v>1</v>
@@ -1970,7 +2016,7 @@
         <v>76</v>
       </c>
       <c r="O21" s="2">
-        <v>3.871389769299662E-259</v>
+        <v>1.0262184891002471E-293</v>
       </c>
       <c r="P21" s="2">
         <v>1</v>
@@ -2065,10 +2111,10 @@
         <v>1.4673724574896321</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>84</v>
+        <v>66</v>
       </c>
       <c r="O23" s="2">
-        <v>1.417594800107819E-140</v>
+        <v>9.2644694952929363E-131</v>
       </c>
       <c r="P23" s="2">
         <v>1</v>
@@ -2076,7 +2122,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
@@ -2091,10 +2137,10 @@
         <v>0.13</v>
       </c>
       <c r="F24" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G24" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>7</v>
@@ -2115,7 +2161,7 @@
         <v>6.05100588265641E-2</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -2126,7 +2172,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -2165,7 +2211,7 @@
         <v>0.91146142395502328</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2">
@@ -2174,7 +2220,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -2189,10 +2235,10 @@
         <v>0.1</v>
       </c>
       <c r="F26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="G26" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>93</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>17</v>
@@ -2213,7 +2259,7 @@
         <v>5.6118629521249928E-2</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2">
@@ -2222,7 +2268,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
@@ -2237,10 +2283,10 @@
         <v>0.06</v>
       </c>
       <c r="F27" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="G27" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="H27" s="2" t="s">
         <v>12</v>
@@ -2270,7 +2316,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
@@ -2285,10 +2331,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="G28" s="2" t="s">
-        <v>100</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>7</v>
@@ -2309,7 +2355,7 @@
         <v>0.87501103163534799</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2">
@@ -2318,7 +2364,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2">
         <v>2</v>
@@ -2333,10 +2379,10 @@
         <v>0.11</v>
       </c>
       <c r="F29" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="G29" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>7</v>
@@ -2357,7 +2403,7 @@
         <v>0.37629948111102729</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2">
@@ -2366,7 +2412,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -2381,10 +2427,10 @@
         <v>0.1</v>
       </c>
       <c r="F30" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="G30" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="G30" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>12</v>
@@ -2405,7 +2451,7 @@
         <v>2.41074373053821E-2</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>43</v>
+        <v>108</v>
       </c>
       <c r="O30" s="2">
         <v>0</v>
@@ -2458,7 +2504,7 @@
         <v>112</v>
       </c>
       <c r="O31" s="2">
-        <v>1.150554359047985E-293</v>
+        <v>1.043498011608572E-296</v>
       </c>
       <c r="P31" s="2">
         <v>1</v>
@@ -2505,7 +2551,7 @@
         <v>5.2674636394968839E-2</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>49</v>
+        <v>116</v>
       </c>
       <c r="O32" s="2"/>
       <c r="P32" s="2">
@@ -2514,7 +2560,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
@@ -2529,10 +2575,10 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>17</v>
@@ -2553,7 +2599,7 @@
         <v>2.2596854997201779E-2</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2">
@@ -2562,7 +2608,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -2577,10 +2623,10 @@
         <v>0.02</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>12</v>
@@ -2601,7 +2647,7 @@
         <v>0.9428557397980063</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="O34" s="2"/>
       <c r="P34" s="2">
@@ -2610,7 +2656,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2">
         <v>2</v>
@@ -2625,10 +2671,10 @@
         <v>0.05</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H35" s="2" t="s">
         <v>7</v>
@@ -2649,10 +2695,10 @@
         <v>7.8403143434910856</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="O35" s="2">
-        <v>3.598839973972987E-107</v>
+        <v>6.3767066151402869E-101</v>
       </c>
       <c r="P35" s="2">
         <v>1</v>
@@ -2660,7 +2706,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -2699,7 +2745,7 @@
         <v>0.61531536549849963</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>101</v>
+        <v>130</v>
       </c>
       <c r="O36" s="2">
         <v>0</v>
@@ -2710,7 +2756,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
@@ -2725,10 +2771,10 @@
         <v>0.09</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H37" s="2" t="s">
         <v>7</v>
@@ -2749,7 +2795,7 @@
         <v>1.907624917534019</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2">
@@ -2758,7 +2804,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B38" s="2">
         <v>2</v>
@@ -2773,10 +2819,10 @@
         <v>0.26</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H38" s="2" t="s">
         <v>17</v>
@@ -2797,7 +2843,7 @@
         <v>0.16162988586917679</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>88</v>
+        <v>45</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2">
@@ -2806,7 +2852,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
@@ -2821,10 +2867,10 @@
         <v>0.06</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H39" s="2" t="s">
         <v>7</v>
@@ -2845,10 +2891,10 @@
         <v>0.11490204463397651</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>45</v>
+        <v>141</v>
       </c>
       <c r="O39" s="2">
-        <v>4.5777537329376068E-166</v>
+        <v>1.126061889321898E-140</v>
       </c>
       <c r="P39" s="2">
         <v>1</v>
@@ -2856,7 +2902,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B40" s="2">
         <v>0</v>
@@ -2895,7 +2941,7 @@
         <v>0.18560580275919461</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>140</v>
+        <v>45</v>
       </c>
       <c r="O40" s="2">
         <v>0</v>
@@ -2906,7 +2952,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>
@@ -2921,10 +2967,10 @@
         <v>0.01</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>17</v>
@@ -2958,11 +3004,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2974,9 +3020,7 @@
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="6" width="27" customWidth="1"/>
     <col min="7" max="7" width="26" customWidth="1"/>
-    <col min="8" max="9" width="10" customWidth="1"/>
-    <col min="10" max="10" width="18" customWidth="1"/>
-    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="8" max="11" width="10" customWidth="1"/>
     <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="10" customWidth="1"/>
     <col min="14" max="14" width="36" customWidth="1"/>
@@ -2989,49 +3033,49 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>179</v>
+        <v>194</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="O1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
@@ -3051,10 +3095,10 @@
         <v>0.25</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>17</v>
@@ -3171,10 +3215,10 @@
         <v>1.691679120530974</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="O4" s="2">
-        <v>7.3632845035759117E-93</v>
+        <v>1.4940295639398831E-82</v>
       </c>
       <c r="P4" s="2">
         <v>1</v>
@@ -3197,7 +3241,7 @@
         <v>0.03</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>48</v>
@@ -3221,10 +3265,10 @@
         <v>3.9324908745388631E-2</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>147</v>
+        <v>58</v>
       </c>
       <c r="O5" s="2">
-        <v>1.52164048184832E-148</v>
+        <v>2.1688246794379609E-129</v>
       </c>
       <c r="P5" s="2">
         <v>1</v>
@@ -3247,7 +3291,7 @@
         <v>0.11</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>29</v>
@@ -3271,7 +3315,7 @@
         <v>0.13260202701536089</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>148</v>
+        <v>166</v>
       </c>
       <c r="O6" s="2"/>
       <c r="P6" s="2">
@@ -3367,7 +3411,7 @@
         <v>5.0227388478100071E-2</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>148</v>
+        <v>33</v>
       </c>
       <c r="O8" s="2">
         <v>0</v>
@@ -3417,10 +3461,10 @@
         <v>0.34188508521068078</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="O9" s="2">
-        <v>1.084939297563064E-157</v>
+        <v>1.423551199907275E-171</v>
       </c>
       <c r="P9" s="2">
         <v>1</v>
@@ -3443,7 +3487,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>42</v>
@@ -3467,7 +3511,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>151</v>
+        <v>49</v>
       </c>
       <c r="O10" s="2">
         <v>0</v>
@@ -3517,7 +3561,7 @@
         <v>5.034153970660727E-2</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>80</v>
+        <v>49</v>
       </c>
       <c r="O11" s="2"/>
       <c r="P11" s="2">
@@ -3565,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="2" t="s">
-        <v>33</v>
+        <v>141</v>
       </c>
       <c r="O12" s="2">
         <v>0</v>
@@ -3615,7 +3659,7 @@
         <v>0.23556750985365399</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>140</v>
+        <v>162</v>
       </c>
       <c r="O13" s="2"/>
       <c r="P13" s="2">
@@ -3663,7 +3707,7 @@
         <v>1.7559255820265991</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>37</v>
+        <v>167</v>
       </c>
       <c r="O14" s="2"/>
       <c r="P14" s="2">
@@ -3672,7 +3716,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="2">
         <v>2</v>
@@ -3711,7 +3755,7 @@
         <v>0.27993181116854671</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="O15" s="2">
         <v>0</v>
@@ -3764,7 +3808,7 @@
         <v>8</v>
       </c>
       <c r="O16" s="2">
-        <v>6.0995240003634923E-254</v>
+        <v>2.8261959658198613E-250</v>
       </c>
       <c r="P16" s="2">
         <v>1</v>
@@ -3811,7 +3855,7 @@
         <v>0.17065730158455639</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2">
@@ -3837,8 +3881,8 @@
       <c r="F18" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>150</v>
+      <c r="G18" s="2">
+        <v>16.329999999999998</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>17</v>
@@ -3859,7 +3903,7 @@
         <v>0.46422982275867919</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>155</v>
+        <v>124</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2">
@@ -3883,10 +3927,10 @@
         <v>0.05</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>7</v>
@@ -3910,7 +3954,7 @@
         <v>156</v>
       </c>
       <c r="O19" s="2">
-        <v>7.635719267002028E-131</v>
+        <v>3.8959303580855849E-131</v>
       </c>
       <c r="P19" s="2">
         <v>1</v>
@@ -3981,10 +4025,10 @@
         <v>0.02</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H21" s="2" t="s">
         <v>7</v>
@@ -4053,7 +4097,7 @@
         <v>4.1100329311271611E-2</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2">
@@ -4101,7 +4145,7 @@
         <v>3.9140045298677283E-2</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2">
@@ -4110,7 +4154,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" s="2">
         <v>2</v>
@@ -4149,7 +4193,7 @@
         <v>0.1153630873568651</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="O24" s="2">
         <v>0</v>
@@ -4160,7 +4204,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B25" s="2">
         <v>0</v>
@@ -4199,7 +4243,7 @@
         <v>0.91146142395502328</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2">
@@ -4208,7 +4252,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -4223,7 +4267,7 @@
         <v>0.12</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>153</v>
@@ -4247,10 +4291,10 @@
         <v>0.117724348488146</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>58</v>
+        <v>33</v>
       </c>
       <c r="O26" s="2">
-        <v>8.1431563273990004E-234</v>
+        <v>5.0603289205340661E-272</v>
       </c>
       <c r="P26" s="2">
         <v>1</v>
@@ -4258,7 +4302,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B27" s="2">
         <v>3</v>
@@ -4297,10 +4341,10 @@
         <v>1.1976669246546909</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>160</v>
+        <v>171</v>
       </c>
       <c r="O27" s="2">
-        <v>5.3546114403975538E-179</v>
+        <v>1.615262237853224E-150</v>
       </c>
       <c r="P27" s="2">
         <v>1</v>
@@ -4308,7 +4352,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B28" s="2">
         <v>1</v>
@@ -4347,7 +4391,7 @@
         <v>0.2460746556637721</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2">
@@ -4356,7 +4400,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="2">
         <v>2</v>
@@ -4371,10 +4415,10 @@
         <v>0.08</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H29" s="2" t="s">
         <v>7</v>
@@ -4395,7 +4439,7 @@
         <v>0.39099413044355902</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2">
@@ -4404,7 +4448,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -4419,10 +4463,10 @@
         <v>0.15</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H30" s="2" t="s">
         <v>12</v>
@@ -4443,7 +4487,7 @@
         <v>2.4085244202157841E-2</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>49</v>
+        <v>173</v>
       </c>
       <c r="O30" s="2">
         <v>0</v>
@@ -4493,10 +4537,10 @@
         <v>1.7283686427944891</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>163</v>
+        <v>174</v>
       </c>
       <c r="O31" s="2">
-        <v>7.3242616472675214E-252</v>
+        <v>8.3709998630918747E-246</v>
       </c>
       <c r="P31" s="2">
         <v>1</v>
@@ -4552,7 +4596,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B33" s="2">
         <v>1</v>
@@ -4591,7 +4635,7 @@
         <v>4.606684906589438E-2</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
       <c r="O33" s="2"/>
       <c r="P33" s="2">
@@ -4600,7 +4644,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B34" s="2">
         <v>0</v>
@@ -4615,10 +4659,10 @@
         <v>0.02</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H34" s="2" t="s">
         <v>12</v>
@@ -4648,7 +4692,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B35" s="2">
         <v>2</v>
@@ -4687,7 +4731,7 @@
         <v>8.68906186840346</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" s="2">
@@ -4696,7 +4740,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B36" s="2">
         <v>0</v>
@@ -4735,7 +4779,7 @@
         <v>0.61531536549849963</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>101</v>
+        <v>161</v>
       </c>
       <c r="O36" s="2">
         <v>0</v>
@@ -4746,7 +4790,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B37" s="2">
         <v>1</v>
@@ -4785,7 +4829,7 @@
         <v>1.9034686591780849</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="O37" s="2"/>
       <c r="P37" s="2">
@@ -4794,7 +4838,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B38" s="2">
         <v>2</v>
@@ -4833,7 +4877,7 @@
         <v>0.30493231998041231</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="O38" s="2"/>
       <c r="P38" s="2">
@@ -4842,7 +4886,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B39" s="2">
         <v>1</v>
@@ -4857,7 +4901,7 @@
         <v>0.06</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>153</v>
@@ -4881,7 +4925,7 @@
         <v>3.4036470580340407E-2</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="O39" s="2"/>
       <c r="P39" s="2">
@@ -4890,7 +4934,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B40" s="2">
         <v>0</v>
@@ -4929,7 +4973,7 @@
         <v>0.18560580275919461</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>169</v>
+        <v>45</v>
       </c>
       <c r="O40" s="2">
         <v>0</v>
@@ -4940,7 +4984,2031 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2</v>
+      </c>
+      <c r="D41" s="2">
+        <v>0.83</v>
+      </c>
+      <c r="E41" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I41" s="2">
+        <v>70</v>
+      </c>
+      <c r="J41" s="2">
+        <v>44</v>
+      </c>
+      <c r="K41" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L41" s="2">
+        <v>0</v>
+      </c>
+      <c r="M41" s="2">
+        <v>0</v>
+      </c>
+      <c r="N41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O41" s="2"/>
+      <c r="P41" s="2">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P41"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P1" sqref="A1:P1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="3" max="3" width="17" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="7" max="7" width="26" customWidth="1"/>
+    <col min="8" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
+    <col min="13" max="13" width="10" customWidth="1"/>
+    <col min="14" max="14" width="36" customWidth="1"/>
+    <col min="15" max="15" width="14" customWidth="1"/>
+    <col min="16" max="16" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.41</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.18</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2">
+        <v>90</v>
+      </c>
+      <c r="J2" s="2">
+        <v>58</v>
+      </c>
+      <c r="K2" s="2">
+        <v>16</v>
+      </c>
+      <c r="L2" s="2">
+        <v>0</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>60</v>
+      </c>
+      <c r="J3" s="2">
+        <v>22</v>
+      </c>
+      <c r="K3" s="2">
+        <v>4096</v>
+      </c>
+      <c r="L3" s="2">
+        <v>0</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="2">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2">
+        <v>29</v>
+      </c>
+      <c r="K4" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L4" s="2">
+        <v>1</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1.6118192079603779</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="O4" s="2">
+        <v>9.6732956587052203E-145</v>
+      </c>
+      <c r="P4" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="2">
+        <v>2</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="2">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2">
+        <v>256</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M5" s="2">
+        <v>3.9324908745388631E-2</v>
+      </c>
+      <c r="N5" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="O5" s="2">
+        <v>4.6961174352982672E-150</v>
+      </c>
+      <c r="P5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="2">
+        <v>10</v>
+      </c>
+      <c r="J6" s="2">
+        <v>5</v>
+      </c>
+      <c r="K6" s="2">
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0</v>
+      </c>
+      <c r="N6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2">
+        <v>80</v>
+      </c>
+      <c r="J7" s="2">
+        <v>41</v>
+      </c>
+      <c r="K7" s="2">
+        <v>3.90625E-3</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E8" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2">
+        <v>70</v>
+      </c>
+      <c r="J8" s="2">
+        <v>48</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0</v>
+      </c>
+      <c r="M8" s="2">
+        <v>5.3833250455082839E-2</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1</v>
+      </c>
+      <c r="C9" s="2">
+        <v>5</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.85</v>
+      </c>
+      <c r="E9" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="2">
+        <v>60</v>
+      </c>
+      <c r="J9" s="2">
+        <v>48</v>
+      </c>
+      <c r="K9" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.34259001271251011</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+      <c r="P9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="2">
+        <v>2</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.65</v>
+      </c>
+      <c r="E10" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="2">
+        <v>40</v>
+      </c>
+      <c r="J10" s="2">
+        <v>30</v>
+      </c>
+      <c r="K10" s="2">
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E11" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I11" s="2">
+        <v>90</v>
+      </c>
+      <c r="J11" s="2">
+        <v>61</v>
+      </c>
+      <c r="K11" s="2">
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.96357921806920577</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="2">
+        <v>0</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="E12" s="2">
+        <v>0.16</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2">
+        <v>70</v>
+      </c>
+      <c r="J12" s="2">
+        <v>64</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L12" s="2">
+        <v>0</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.30931506202357739</v>
+      </c>
+      <c r="N12" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2">
+        <v>30</v>
+      </c>
+      <c r="J13" s="2">
+        <v>30</v>
+      </c>
+      <c r="K13" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.23556750985365399</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="2">
+        <v>0</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.67</v>
+      </c>
+      <c r="E14" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="2">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
+        <v>8</v>
+      </c>
+      <c r="K14" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0</v>
+      </c>
+      <c r="M14" s="2">
+        <v>1.7559255820265991</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="O14" s="2"/>
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" s="2">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E15" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="2">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
+        <v>10</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L15" s="2">
+        <v>1</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.17326091192550669</v>
+      </c>
+      <c r="N15" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+      <c r="P15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2">
+        <v>5</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.52</v>
+      </c>
+      <c r="E16" s="2">
+        <v>0.22</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2">
+        <v>80</v>
+      </c>
+      <c r="J16" s="2">
+        <v>48</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.54783469762416892</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="O16" s="2">
+        <v>8.1111277817366916E-187</v>
+      </c>
+      <c r="P16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="2">
+        <v>2</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2">
+        <v>30</v>
+      </c>
+      <c r="J17" s="2">
+        <v>13</v>
+      </c>
+      <c r="K17" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.17065730158455639</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="O17" s="2"/>
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="2">
+        <v>3</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3</v>
+      </c>
+      <c r="D18" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E18" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I18" s="2">
+        <v>40</v>
+      </c>
+      <c r="J18" s="2">
+        <v>39</v>
+      </c>
+      <c r="K18" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.66087587563379036</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="O18" s="2">
+        <v>1.15604418421361E-60</v>
+      </c>
+      <c r="P18" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B19" s="2">
+        <v>1</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E19" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I19" s="2">
+        <v>70</v>
+      </c>
+      <c r="J19" s="2">
+        <v>52</v>
+      </c>
+      <c r="K19" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.86146163867615289</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" s="2">
+        <v>1.4958687694259799E-130</v>
+      </c>
+      <c r="P19" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>3</v>
+      </c>
+      <c r="D20" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="E20" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I20" s="2">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
+        <v>10</v>
+      </c>
+      <c r="K20" s="2">
+        <v>2.44140625E-4</v>
+      </c>
+      <c r="L20" s="2">
+        <v>0</v>
+      </c>
+      <c r="M20" s="2">
+        <v>0</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E21" s="2">
+        <v>0.05</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I21" s="2">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
+        <v>4</v>
+      </c>
+      <c r="K21" s="2">
+        <v>4096</v>
+      </c>
+      <c r="L21" s="2">
+        <v>0</v>
+      </c>
+      <c r="M21" s="2">
+        <v>8.4781343983008406E-2</v>
+      </c>
+      <c r="N21" s="2" t="s">
         <v>141</v>
+      </c>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="2">
+        <v>3</v>
+      </c>
+      <c r="C22" s="2">
+        <v>4</v>
+      </c>
+      <c r="D22" s="2">
+        <v>0.78</v>
+      </c>
+      <c r="E22" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="2">
+        <v>50</v>
+      </c>
+      <c r="J22" s="2">
+        <v>46</v>
+      </c>
+      <c r="K22" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L22" s="2">
+        <v>0</v>
+      </c>
+      <c r="M22" s="2">
+        <v>4.1100329311271611E-2</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B23" s="2">
+        <v>1</v>
+      </c>
+      <c r="C23" s="2">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="E23" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I23" s="2">
+        <v>90</v>
+      </c>
+      <c r="J23" s="2">
+        <v>59</v>
+      </c>
+      <c r="K23" s="2">
+        <v>16</v>
+      </c>
+      <c r="L23" s="2">
+        <v>0</v>
+      </c>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="B24" s="2">
+        <v>2</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>0.51</v>
+      </c>
+      <c r="E24" s="2">
+        <v>0.31</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="2">
+        <v>20</v>
+      </c>
+      <c r="J24" s="2">
+        <v>19</v>
+      </c>
+      <c r="K24" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L24" s="2">
+        <v>0</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="2">
+        <v>0</v>
+      </c>
+      <c r="C25" s="2">
+        <v>2</v>
+      </c>
+      <c r="D25" s="2">
+        <v>0.53</v>
+      </c>
+      <c r="E25" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" s="2">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
+        <v>6</v>
+      </c>
+      <c r="K25" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0.49696986842121238</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="O25" s="2">
+        <v>4.5258255753011802E-210</v>
+      </c>
+      <c r="P25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <v>0.63</v>
+      </c>
+      <c r="E26" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I26" s="2">
+        <v>20</v>
+      </c>
+      <c r="J26" s="2">
+        <v>12</v>
+      </c>
+      <c r="K26" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
+      <c r="M26" s="2">
+        <v>0.1160170938891967</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="O26" s="2"/>
+      <c r="P26" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" s="2">
+        <v>3</v>
+      </c>
+      <c r="C27" s="2">
+        <v>4</v>
+      </c>
+      <c r="D27" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="2">
+        <v>40</v>
+      </c>
+      <c r="J27" s="2">
+        <v>31</v>
+      </c>
+      <c r="K27" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L27" s="2">
+        <v>0</v>
+      </c>
+      <c r="M27" s="2">
+        <v>3.8947565445306941E-2</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="O27" s="2"/>
+      <c r="P27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1</v>
+      </c>
+      <c r="C28" s="2">
+        <v>4</v>
+      </c>
+      <c r="D28" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="E28" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I28" s="2">
+        <v>10</v>
+      </c>
+      <c r="J28" s="2">
+        <v>6</v>
+      </c>
+      <c r="K28" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M28" s="2">
+        <v>0.92310299630094039</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="O28" s="2"/>
+      <c r="P28" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="2">
+        <v>4</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0.74</v>
+      </c>
+      <c r="E29" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I29" s="2">
+        <v>10</v>
+      </c>
+      <c r="J29" s="2">
+        <v>8</v>
+      </c>
+      <c r="K29" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L29" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M29" s="2">
+        <v>0.84661050989247588</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O29" s="2"/>
+      <c r="P29" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="E30" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I30" s="2">
+        <v>80</v>
+      </c>
+      <c r="J30" s="2">
+        <v>60</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L30" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="O30" s="2">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1</v>
+      </c>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="E31" s="2">
+        <v>0.04</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I31" s="2">
+        <v>90</v>
+      </c>
+      <c r="J31" s="2">
+        <v>76</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1</v>
+      </c>
+      <c r="L31" s="2">
+        <v>0</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O31" s="2"/>
+      <c r="P31" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B32" s="2">
+        <v>1</v>
+      </c>
+      <c r="C32" s="2">
+        <v>2</v>
+      </c>
+      <c r="D32" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="E32" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I32" s="2">
+        <v>30</v>
+      </c>
+      <c r="J32" s="2">
+        <v>22</v>
+      </c>
+      <c r="K32" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L32" s="2">
+        <v>0</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O32" s="2"/>
+      <c r="P32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="B33" s="2">
+        <v>1</v>
+      </c>
+      <c r="C33" s="2">
+        <v>4</v>
+      </c>
+      <c r="D33" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="E33" s="2">
+        <v>0.02</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I33" s="2">
+        <v>10</v>
+      </c>
+      <c r="J33" s="2">
+        <v>9</v>
+      </c>
+      <c r="K33" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L33" s="2">
+        <v>0</v>
+      </c>
+      <c r="M33" s="2">
+        <v>2.3211622675995199E-2</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="O33" s="2"/>
+      <c r="P33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B34" s="2">
+        <v>0</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>0.47</v>
+      </c>
+      <c r="E34" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I34" s="2">
+        <v>10</v>
+      </c>
+      <c r="J34" s="2">
+        <v>9</v>
+      </c>
+      <c r="K34" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L34" s="2">
+        <v>0</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.33702804965341249</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O34" s="2"/>
+      <c r="P34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0.48</v>
+      </c>
+      <c r="E35" s="2">
+        <v>0.03</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="2">
+        <v>10</v>
+      </c>
+      <c r="J35" s="2">
+        <v>10</v>
+      </c>
+      <c r="K35" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L35" s="2">
+        <v>0</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1.0158778981757439</v>
+      </c>
+      <c r="N35" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="O35" s="2"/>
+      <c r="P35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B36" s="2">
+        <v>0</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2">
+        <v>40</v>
+      </c>
+      <c r="J36" s="2">
+        <v>13</v>
+      </c>
+      <c r="K36" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.61531536549849963</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="O36" s="2">
+        <v>0</v>
+      </c>
+      <c r="P36" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="E37" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I37" s="2">
+        <v>20</v>
+      </c>
+      <c r="J37" s="2">
+        <v>14</v>
+      </c>
+      <c r="K37" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L37" s="2">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="M37" s="2">
+        <v>1.9034686591780849</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B38" s="2">
+        <v>2</v>
+      </c>
+      <c r="C38" s="2">
+        <v>3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I38" s="2">
+        <v>10</v>
+      </c>
+      <c r="J38" s="2">
+        <v>10</v>
+      </c>
+      <c r="K38" s="2">
+        <v>9.5367431640625E-7</v>
+      </c>
+      <c r="L38" s="2">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="M38" s="2">
+        <v>1.1131865851591649</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="O38" s="2">
+        <v>1.524392454176867E-6</v>
+      </c>
+      <c r="P38" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1</v>
+      </c>
+      <c r="C39" s="2">
+        <v>5</v>
+      </c>
+      <c r="D39" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="E39" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I39" s="2">
+        <v>90</v>
+      </c>
+      <c r="J39" s="2">
+        <v>48</v>
+      </c>
+      <c r="K39" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L39" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M39" s="2">
+        <v>0.57342013318555141</v>
+      </c>
+      <c r="N39" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B40" s="2">
+        <v>0</v>
+      </c>
+      <c r="C40" s="2">
+        <v>4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="2">
+        <v>10</v>
+      </c>
+      <c r="J40" s="2">
+        <v>6</v>
+      </c>
+      <c r="K40" s="2">
+        <v>1.52587890625E-5</v>
+      </c>
+      <c r="L40" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M40" s="2">
+        <v>0.18560580275919461</v>
+      </c>
+      <c r="N40" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="O40" s="2">
+        <v>0</v>
+      </c>
+      <c r="P40" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>143</v>
       </c>
       <c r="B41" s="2">
         <v>1</v>

</xml_diff>